<commit_message>
Conversión a PDF de los archivos de Excel
</commit_message>
<xml_diff>
--- a/Build-First-Automation-StudioX/First Automation Using Microsoft Office/Invoices/Invoice 1.xlsx
+++ b/Build-First-Automation-StudioX/First Automation Using Microsoft Office/Invoices/Invoice 1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bianca.dragu\Documents\03. RPA Starter\2022.10 Build Your First Automation with StudioX\Invoices - Working Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\UiPath-Academy\Build-First-Automation-StudioX\First Automation Using Microsoft Office\Invoices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A622768D-4E4F-4752-A082-92A9534287D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8089386D-0FC6-4601-A374-DCE1F8FA446A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{ACCB1FA6-7E67-4590-BB25-A17FCE65C786}"/>
+    <workbookView xWindow="1080" yWindow="2325" windowWidth="15375" windowHeight="7785" xr2:uid="{ACCB1FA6-7E67-4590-BB25-A17FCE65C786}"/>
   </bookViews>
   <sheets>
     <sheet name="Invoice" sheetId="1" r:id="rId1"/>
@@ -123,14 +123,15 @@
     <t>CLIENT CODE</t>
   </si>
   <si>
-    <t>name, email address</t>
+    <t>Charlie, charlie@mail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.000%"/>
@@ -412,7 +413,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -503,18 +504,51 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -522,38 +556,9 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="6" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -581,9 +586,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -621,7 +626,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -727,7 +732,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -869,7 +874,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -883,29 +888,29 @@
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" customWidth="1"/>
-    <col min="3" max="3" width="19.44140625" customWidth="1"/>
-    <col min="4" max="4" width="4.5546875" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" customWidth="1"/>
-    <col min="6" max="6" width="21.109375" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="4.5703125" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="46.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:6" ht="46.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="30" t="s">
         <v>21</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="2"/>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="30"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F1" s="41"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>23</v>
       </c>
@@ -915,7 +920,7 @@
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>24</v>
       </c>
@@ -925,21 +930,21 @@
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
-      <c r="D4" s="32" t="s">
+      <c r="D4" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="32"/>
-      <c r="F4" s="33" t="s">
+      <c r="E4" s="42"/>
+      <c r="F4" s="31" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -951,7 +956,7 @@
         <v>44329</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
@@ -959,21 +964,21 @@
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="34" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="35"/>
+      <c r="B7" s="46"/>
       <c r="C7" s="29"/>
-      <c r="D7" s="32" t="s">
+      <c r="D7" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="32"/>
-      <c r="F7" s="33" t="s">
+      <c r="E7" s="42"/>
+      <c r="F7" s="31" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>2</v>
       </c>
@@ -987,7 +992,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
@@ -997,7 +1002,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>5</v>
       </c>
@@ -1007,7 +1012,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>6</v>
       </c>
@@ -1017,7 +1022,7 @@
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>7</v>
       </c>
@@ -1027,7 +1032,7 @@
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>8</v>
       </c>
@@ -1037,7 +1042,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
@@ -1045,23 +1050,23 @@
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="37" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="37"/>
+      <c r="B15" s="33"/>
       <c r="C15" s="28"/>
-      <c r="D15" s="36" t="s">
+      <c r="D15" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="36" t="s">
+      <c r="E15" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="36" t="s">
+      <c r="F15" s="32" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="17.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="24" t="s">
         <v>13</v>
       </c>
@@ -1078,7 +1083,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
         <v>14</v>
       </c>
@@ -1095,21 +1100,21 @@
         <v>875</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="20.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="20.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
         <v>15</v>
       </c>
       <c r="B18" s="25"/>
       <c r="C18" s="25"/>
       <c r="D18" s="21"/>
-      <c r="E18" s="18">
-        <v>1</v>
+      <c r="E18" s="47">
+        <v>100</v>
       </c>
       <c r="F18" s="19">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="25"/>
       <c r="B19" s="25"/>
       <c r="C19" s="25"/>
@@ -1120,7 +1125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="23"/>
       <c r="B20" s="23"/>
       <c r="C20" s="23"/>
@@ -1131,22 +1136,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="46" t="s">
+    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="B21" s="46"/>
-      <c r="C21" s="46"/>
-      <c r="D21" s="38" t="s">
+      <c r="B21" s="43"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="44" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="38"/>
-      <c r="F21" s="42">
+      <c r="E21" s="44"/>
+      <c r="F21" s="35">
         <f>F16+F17-F18</f>
         <v>1074</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
       <c r="B22" s="13"/>
       <c r="C22" s="13"/>
@@ -1154,37 +1159,37 @@
         <v>18</v>
       </c>
       <c r="E22" s="39"/>
-      <c r="F22" s="43">
+      <c r="F22" s="36">
         <v>4.2500000000000003E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="12"/>
       <c r="B23" s="13"/>
       <c r="C23" s="13"/>
-      <c r="D23" s="40" t="s">
+      <c r="D23" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="E23" s="40"/>
-      <c r="F23" s="44">
+      <c r="E23" s="34"/>
+      <c r="F23" s="37">
         <f>F21*F22</f>
         <v>45.645000000000003</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
       <c r="B24" s="13"/>
       <c r="C24" s="13"/>
-      <c r="D24" s="41" t="s">
+      <c r="D24" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="E24" s="41"/>
-      <c r="F24" s="45">
+      <c r="E24" s="40"/>
+      <c r="F24" s="38">
         <f>F21+F23</f>
         <v>1119.645</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
@@ -1192,7 +1197,7 @@
       <c r="E25" s="14"/>
       <c r="F25" s="14"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
@@ -1200,7 +1205,7 @@
       <c r="E26" s="9"/>
       <c r="F26" s="9"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="15"/>
       <c r="B27" s="15"/>
       <c r="C27" s="15"/>
@@ -1208,7 +1213,7 @@
       <c r="E27" s="15"/>
       <c r="F27" s="15"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="15"/>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
@@ -1216,7 +1221,7 @@
       <c r="E28" s="15"/>
       <c r="F28" s="15"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="15"/>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
@@ -1224,7 +1229,7 @@
       <c r="E29" s="15"/>
       <c r="F29" s="15"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="15"/>
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
@@ -1232,7 +1237,7 @@
       <c r="E30" s="15"/>
       <c r="F30" s="15"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="27" t="s">
         <v>29</v>
       </c>
@@ -1242,7 +1247,7 @@
       <c r="E31" s="27"/>
       <c r="F31" s="27"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
@@ -1252,14 +1257,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="A7:B7"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="D24:E24"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="D7:E7"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="A7:B7"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1" xr:uid="{3973258D-70B0-4F2B-9A52-AA2F46F0125B}">

</xml_diff>